<commit_message>
added kerber network example, added time series information, adjusted code structure, fixed bug on template files, now everything is working
</commit_message>
<xml_diff>
--- a/template_topology.xlsx
+++ b/template_topology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED88B0D-F664-6141-963A-F46994615037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF2F91C-9D50-C544-B920-C03C60679BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="173">
   <si>
     <t>version</t>
   </si>
@@ -426,9 +426,6 @@
     <t>int64</t>
   </si>
   <si>
-    <t>int32</t>
-  </si>
-  <si>
     <t>rft_pu</t>
   </si>
   <si>
@@ -466,6 +463,90 @@
   </si>
   <si>
     <t>max_q_to_mvar</t>
+  </si>
+  <si>
+    <t>sgen</t>
+  </si>
+  <si>
+    <t>current_source</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>soc_percent</t>
+  </si>
+  <si>
+    <t>min_e_mwh</t>
+  </si>
+  <si>
+    <t>max_e_mwh</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>min_q_mvar</t>
+  </si>
+  <si>
+    <t>max_q_mvar</t>
+  </si>
+  <si>
+    <t>slack</t>
+  </si>
+  <si>
+    <t>power_station_trafo</t>
+  </si>
+  <si>
+    <t>trafo3w</t>
+  </si>
+  <si>
+    <t>mv_bus</t>
+  </si>
+  <si>
+    <t>sn_hv_mva</t>
+  </si>
+  <si>
+    <t>sn_mv_mva</t>
+  </si>
+  <si>
+    <t>sn_lv_mva</t>
+  </si>
+  <si>
+    <t>vn_mv_kv</t>
+  </si>
+  <si>
+    <t>vk_hv_percent</t>
+  </si>
+  <si>
+    <t>vk_mv_percent</t>
+  </si>
+  <si>
+    <t>vk_lv_percent</t>
+  </si>
+  <si>
+    <t>vkr_hv_percent</t>
+  </si>
+  <si>
+    <t>vkr_mv_percent</t>
+  </si>
+  <si>
+    <t>vkr_lv_percent</t>
+  </si>
+  <si>
+    <t>shift_mv_degree</t>
+  </si>
+  <si>
+    <t>shift_lv_degree</t>
+  </si>
+  <si>
+    <t>tap_at_star_point</t>
+  </si>
+  <si>
+    <t>impedance</t>
+  </si>
+  <si>
+    <t>dcline</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0177EE3-CE95-7A42-A901-D0BE5A38614F}">
   <dimension ref="B1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
@@ -1257,16 +1338,16 @@
         <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -1304,31 +1385,31 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>138</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>139</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>140</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>141</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>142</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>143</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>144</v>
-      </c>
-      <c r="N1" t="s">
-        <v>145</v>
       </c>
       <c r="O1" t="s">
         <v>10</v>
@@ -2773,10 +2854,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3007,13 +3088,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3021,10 +3102,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3035,13 +3116,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3049,13 +3130,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3063,13 +3144,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3077,13 +3158,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C22" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3091,13 +3172,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3105,13 +3186,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3119,13 +3200,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3133,13 +3214,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3147,13 +3228,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3161,10 +3242,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
         <v>128</v>
@@ -3175,10 +3256,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D29" t="s">
         <v>128</v>
@@ -3189,13 +3270,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3203,13 +3284,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3217,13 +3298,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>149</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3231,13 +3312,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>150</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3245,13 +3326,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3259,13 +3340,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3273,13 +3354,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3287,13 +3368,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3301,13 +3382,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3315,10 +3396,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
         <v>128</v>
@@ -3329,10 +3410,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>128</v>
@@ -3343,10 +3424,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
         <v>128</v>
@@ -3357,13 +3438,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="D42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3371,13 +3452,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3385,13 +3466,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3399,13 +3480,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3413,13 +3494,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3427,13 +3508,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3441,13 +3522,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -3455,10 +3536,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>155</v>
       </c>
       <c r="D49" t="s">
         <v>128</v>
@@ -3469,13 +3550,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -3483,13 +3564,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -3497,13 +3578,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -3511,13 +3592,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -3525,13 +3606,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -3539,13 +3620,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -3553,10 +3634,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D56" t="s">
         <v>128</v>
@@ -3567,13 +3648,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D57" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -3581,13 +3662,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -3595,13 +3676,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -3609,13 +3690,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C60" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D60" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -3623,10 +3704,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
         <v>128</v>
@@ -3637,10 +3718,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
         <v>128</v>
@@ -3651,13 +3732,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3665,13 +3746,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -3679,13 +3760,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -3693,13 +3774,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D66" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -3707,13 +3788,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D67" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3721,10 +3802,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D68" t="s">
         <v>128</v>
@@ -3735,10 +3816,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D69" t="s">
         <v>128</v>
@@ -3749,12 +3830,1216 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C70" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" t="s">
+        <v>37</v>
+      </c>
+      <c r="D71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>124</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C74" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>124</v>
+      </c>
+      <c r="C75" t="s">
+        <v>41</v>
+      </c>
+      <c r="D75" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>124</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>124</v>
+      </c>
+      <c r="C77" t="s">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>125</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>125</v>
+      </c>
+      <c r="C81" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>125</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" t="s">
+        <v>48</v>
+      </c>
+      <c r="D83" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" t="s">
+        <v>50</v>
+      </c>
+      <c r="D85" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>125</v>
+      </c>
+      <c r="C86" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>125</v>
+      </c>
+      <c r="C87" t="s">
+        <v>52</v>
+      </c>
+      <c r="D87" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>125</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D88" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" t="s">
+        <v>54</v>
+      </c>
+      <c r="D89" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>125</v>
+      </c>
+      <c r="C90" t="s">
+        <v>55</v>
+      </c>
+      <c r="D90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91" t="s">
+        <v>56</v>
+      </c>
+      <c r="D91" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" t="s">
+        <v>57</v>
+      </c>
+      <c r="D92" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D93" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>125</v>
+      </c>
+      <c r="C94" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>125</v>
+      </c>
+      <c r="C95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D95" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>125</v>
+      </c>
+      <c r="C96" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>125</v>
+      </c>
+      <c r="C97" t="s">
+        <v>62</v>
+      </c>
+      <c r="D97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>125</v>
+      </c>
+      <c r="C98" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>125</v>
+      </c>
+      <c r="C99" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>125</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+      <c r="D100" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>156</v>
+      </c>
+      <c r="C101" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>156</v>
+      </c>
+      <c r="C102" t="s">
+        <v>31</v>
+      </c>
+      <c r="D102" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>156</v>
+      </c>
+      <c r="C103" t="s">
+        <v>46</v>
+      </c>
+      <c r="D103" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>156</v>
+      </c>
+      <c r="C104" t="s">
+        <v>157</v>
+      </c>
+      <c r="D104" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>156</v>
+      </c>
+      <c r="C105" t="s">
+        <v>47</v>
+      </c>
+      <c r="D105" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>156</v>
+      </c>
+      <c r="C106" t="s">
+        <v>158</v>
+      </c>
+      <c r="D106" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>156</v>
+      </c>
+      <c r="C107" t="s">
+        <v>159</v>
+      </c>
+      <c r="D107" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>156</v>
+      </c>
+      <c r="C108" t="s">
+        <v>160</v>
+      </c>
+      <c r="D108" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>156</v>
+      </c>
+      <c r="C109" t="s">
+        <v>48</v>
+      </c>
+      <c r="D109" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>156</v>
+      </c>
+      <c r="C110" t="s">
+        <v>161</v>
+      </c>
+      <c r="D110" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>156</v>
+      </c>
+      <c r="C111" t="s">
+        <v>49</v>
+      </c>
+      <c r="D111" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>156</v>
+      </c>
+      <c r="C112" t="s">
+        <v>162</v>
+      </c>
+      <c r="D112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>156</v>
+      </c>
+      <c r="C113" t="s">
+        <v>163</v>
+      </c>
+      <c r="D113" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>156</v>
+      </c>
+      <c r="C114" t="s">
+        <v>164</v>
+      </c>
+      <c r="D114" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>156</v>
+      </c>
+      <c r="C115" t="s">
+        <v>165</v>
+      </c>
+      <c r="D115" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>156</v>
+      </c>
+      <c r="C116" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>156</v>
+      </c>
+      <c r="C117" t="s">
+        <v>167</v>
+      </c>
+      <c r="D117" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>156</v>
+      </c>
+      <c r="C118" t="s">
+        <v>52</v>
+      </c>
+      <c r="D118" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>156</v>
+      </c>
+      <c r="C119" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>156</v>
+      </c>
+      <c r="C120" t="s">
+        <v>168</v>
+      </c>
+      <c r="D120" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>156</v>
+      </c>
+      <c r="C121" t="s">
+        <v>169</v>
+      </c>
+      <c r="D121" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>156</v>
+      </c>
+      <c r="C122" t="s">
+        <v>55</v>
+      </c>
+      <c r="D122" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>156</v>
+      </c>
+      <c r="C123" t="s">
+        <v>56</v>
+      </c>
+      <c r="D123" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>156</v>
+      </c>
+      <c r="C124" t="s">
+        <v>57</v>
+      </c>
+      <c r="D124" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>156</v>
+      </c>
+      <c r="C125" t="s">
+        <v>58</v>
+      </c>
+      <c r="D125" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>156</v>
+      </c>
+      <c r="C126" t="s">
+        <v>59</v>
+      </c>
+      <c r="D126" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>156</v>
+      </c>
+      <c r="C127" t="s">
+        <v>60</v>
+      </c>
+      <c r="D127" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
         <v>126</v>
       </c>
-      <c r="C70" t="s">
+      <c r="B128" t="s">
+        <v>156</v>
+      </c>
+      <c r="C128" t="s">
+        <v>61</v>
+      </c>
+      <c r="D128" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>156</v>
+      </c>
+      <c r="C129" t="s">
+        <v>170</v>
+      </c>
+      <c r="D129" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>156</v>
+      </c>
+      <c r="C130" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" t="s">
+        <v>3</v>
+      </c>
+      <c r="D131" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>171</v>
+      </c>
+      <c r="C132" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>171</v>
+      </c>
+      <c r="C133" t="s">
+        <v>33</v>
+      </c>
+      <c r="D133" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>171</v>
+      </c>
+      <c r="C134" t="s">
+        <v>132</v>
+      </c>
+      <c r="D134" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>171</v>
+      </c>
+      <c r="C135" t="s">
+        <v>133</v>
+      </c>
+      <c r="D135" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>171</v>
+      </c>
+      <c r="C136" t="s">
+        <v>134</v>
+      </c>
+      <c r="D136" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>171</v>
+      </c>
+      <c r="C137" t="s">
+        <v>135</v>
+      </c>
+      <c r="D137" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>171</v>
+      </c>
+      <c r="C138" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>171</v>
+      </c>
+      <c r="C139" t="s">
+        <v>10</v>
+      </c>
+      <c r="D139" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>172</v>
+      </c>
+      <c r="C140" t="s">
+        <v>3</v>
+      </c>
+      <c r="D140" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>172</v>
+      </c>
+      <c r="C141" t="s">
+        <v>32</v>
+      </c>
+      <c r="D141" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>172</v>
+      </c>
+      <c r="C142" t="s">
+        <v>33</v>
+      </c>
+      <c r="D142" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>172</v>
+      </c>
+      <c r="C143" t="s">
+        <v>17</v>
+      </c>
+      <c r="D143" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>172</v>
+      </c>
+      <c r="C144" t="s">
+        <v>136</v>
+      </c>
+      <c r="D144" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>172</v>
+      </c>
+      <c r="C145" t="s">
+        <v>137</v>
+      </c>
+      <c r="D145" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>172</v>
+      </c>
+      <c r="C146" t="s">
+        <v>138</v>
+      </c>
+      <c r="D146" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>172</v>
+      </c>
+      <c r="C147" t="s">
+        <v>139</v>
+      </c>
+      <c r="D147" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>172</v>
+      </c>
+      <c r="C148" t="s">
+        <v>140</v>
+      </c>
+      <c r="D148" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>172</v>
+      </c>
+      <c r="C149" t="s">
+        <v>141</v>
+      </c>
+      <c r="D149" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>172</v>
+      </c>
+      <c r="C150" t="s">
+        <v>142</v>
+      </c>
+      <c r="D150" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>172</v>
+      </c>
+      <c r="C151" t="s">
+        <v>143</v>
+      </c>
+      <c r="D151" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>172</v>
+      </c>
+      <c r="C152" t="s">
+        <v>144</v>
+      </c>
+      <c r="D152" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>172</v>
+      </c>
+      <c r="C153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>126</v>
+      </c>
+      <c r="C154" t="s">
+        <v>63</v>
+      </c>
+      <c r="D154" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>126</v>
+      </c>
+      <c r="C155" t="s">
+        <v>64</v>
+      </c>
+      <c r="D155" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>126</v>
+      </c>
+      <c r="C156" t="s">
         <v>65</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D156" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>